<commit_message>
Update cac tinh nang va sua loi lan 2
</commit_message>
<xml_diff>
--- a/public/temp/evaluation_summary_03_2025.xlsx
+++ b/public/temp/evaluation_summary_03_2025.xlsx
@@ -596,10 +596,14 @@
         <v>18</v>
       </c>
       <c r="E5" s="4">
-        <v>62</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
         <v>19</v>
@@ -813,13 +817,13 @@
         <v>85.2</v>
       </c>
       <c r="L12" s="4">
-        <v>75.0</v>
+        <v>80.0</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="N12" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cập nhật và sửa lỗi chức năng
</commit_message>
<xml_diff>
--- a/public/temp/evaluation_summary_03_2025.xlsx
+++ b/public/temp/evaluation_summary_03_2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>TỔNG HỢP Kết quả đánh giá, xếp loại chất lượng công chức</t>
   </si>
@@ -65,61 +65,85 @@
     <t>Tổng Nhiệm Vụ</t>
   </si>
   <si>
-    <t>Chan Dan</t>
+    <t>Nguyễn Đình Long</t>
+  </si>
+  <si>
+    <t>Chi cục phó</t>
+  </si>
+  <si>
+    <t>Nghiệp vụ</t>
+  </si>
+  <si>
+    <t>Không đánh giá</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Khánh</t>
+  </si>
+  <si>
+    <t>Đội trưởng</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Lê Văn Thành</t>
+  </si>
+  <si>
+    <t>Đội phó</t>
+  </si>
+  <si>
+    <t>Nguyễn Thành Đạt</t>
+  </si>
+  <si>
+    <t>Bùi Tú</t>
+  </si>
+  <si>
+    <t>Công chức</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Bùi Thanh San</t>
   </si>
   <si>
     <t>Chi cục trưởng</t>
   </si>
   <si>
-    <t>Nghiệp vụ</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Nguyễn Duy Cường</t>
-  </si>
-  <si>
-    <t>Chi cục phó</t>
+    <t>Phòng Tổ chức cán bộ</t>
+  </si>
+  <si>
+    <t>Đào Xuân An</t>
+  </si>
+  <si>
+    <t>Trưởng phòng</t>
+  </si>
+  <si>
+    <t>Nguyễn Trí Dũng</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Liên</t>
+  </si>
+  <si>
+    <t>Biện Thị Hoài</t>
+  </si>
+  <si>
+    <t>Minh Phương</t>
+  </si>
+  <si>
+    <t>Chánh Văn phòng</t>
+  </si>
+  <si>
+    <t>Văn phòng</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>Hoàng Văn Nam</t>
-  </si>
-  <si>
-    <t>Đội trưởng</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Hải</t>
-  </si>
-  <si>
-    <t>Đội phó</t>
-  </si>
-  <si>
-    <t>Nguyễn Thành Đạt</t>
-  </si>
-  <si>
-    <t>Minh Phương</t>
-  </si>
-  <si>
-    <t>Chánh Văn phòng</t>
-  </si>
-  <si>
-    <t>Văn phòng</t>
-  </si>
-  <si>
     <t>Phan Nghĩa</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Nguyễn Hiếu</t>
-  </si>
-  <si>
-    <t>Công chức</t>
   </si>
 </sst>
 </file>
@@ -504,10 +528,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4:N12"/>
+      <selection activeCell="A4" sqref="A4:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -595,30 +619,18 @@
       <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4">
-        <v>25</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4">
-        <v>50.0</v>
-      </c>
+      <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="4">
-        <v>2</v>
-      </c>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="4">
@@ -639,12 +651,16 @@
         <v>22</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4">
+        <v>60</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="4">
@@ -661,20 +677,14 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4">
-        <v>60</v>
-      </c>
+      <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="4">
-        <v>1</v>
-      </c>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="4">
@@ -684,21 +694,19 @@
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N8" s="4"/>
     </row>
@@ -707,10 +715,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -718,46 +726,56 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="L9" s="4">
+        <v>100.0</v>
+      </c>
       <c r="M9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4">
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E10" s="4">
+        <v>25</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="4">
-        <v>40</v>
-      </c>
-      <c r="L10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
+        <v>66.67</v>
+      </c>
       <c r="M10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="N10" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -765,64 +783,210 @@
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>28</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="4">
-        <v>100</v>
-      </c>
-      <c r="L11" s="4">
-        <v>100.0</v>
-      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
       <c r="M11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="4">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="4">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="4">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4">
         <v>22</v>
       </c>
-      <c r="J12" s="4">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="4">
+        <v>100</v>
+      </c>
+      <c r="K14" s="4">
+        <v>95</v>
+      </c>
+      <c r="L14" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="4">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4">
+        <v>40</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="4">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4">
+        <v>100</v>
+      </c>
+      <c r="L16" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="4">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="4">
         <v>97.5</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K17" s="4">
         <v>85.2</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L17" s="4">
         <v>80.0</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="4">
+      <c r="M17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="4">
         <v>5</v>
       </c>
     </row>
@@ -831,7 +995,8 @@
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="D5:D9"/>
-    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="D15:D17"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sửa và cập nhật chức năng
</commit_message>
<xml_diff>
--- a/public/temp/evaluation_summary_03_2025.xlsx
+++ b/public/temp/evaluation_summary_03_2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>TỔNG HỢP Kết quả đánh giá, xếp loại chất lượng công chức</t>
   </si>
@@ -65,33 +65,30 @@
     <t>Tổng Nhiệm Vụ</t>
   </si>
   <si>
-    <t>Nguyễn Đình Long</t>
-  </si>
-  <si>
-    <t>Chi cục phó</t>
+    <t>Nguyễn Văn Khánh</t>
+  </si>
+  <si>
+    <t>Đội trưởng</t>
   </si>
   <si>
     <t>Nghiệp vụ</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Lê Văn Thành</t>
+  </si>
+  <si>
+    <t>Đội phó</t>
+  </si>
+  <si>
     <t>Không đánh giá</t>
   </si>
   <si>
-    <t>Nguyễn Văn Khánh</t>
-  </si>
-  <si>
-    <t>Đội trưởng</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Lê Văn Thành</t>
-  </si>
-  <si>
-    <t>Đội phó</t>
-  </si>
-  <si>
     <t>Nguyễn Thành Đạt</t>
   </si>
   <si>
@@ -101,49 +98,13 @@
     <t>Công chức</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Bùi Thanh San</t>
-  </si>
-  <si>
-    <t>Chi cục trưởng</t>
-  </si>
-  <si>
-    <t>Phòng Tổ chức cán bộ</t>
-  </si>
-  <si>
-    <t>Đào Xuân An</t>
-  </si>
-  <si>
-    <t>Trưởng phòng</t>
-  </si>
-  <si>
-    <t>Nguyễn Trí Dũng</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Liên</t>
-  </si>
-  <si>
-    <t>Biện Thị Hoài</t>
-  </si>
-  <si>
-    <t>Minh Phương</t>
-  </si>
-  <si>
-    <t>Chánh Văn phòng</t>
+    <t>Nguyễn Hiếu</t>
   </si>
   <si>
     <t>Văn phòng</t>
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>Phan Nghĩa</t>
-  </si>
-  <si>
-    <t>Nguyễn Hiếu</t>
   </si>
 </sst>
 </file>
@@ -528,10 +489,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4:N17"/>
+      <selection activeCell="A4" sqref="A4:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -623,54 +584,54 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="4">
+        <v>60</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="4">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="4">
-        <v>60</v>
-      </c>
+      <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="4">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="4">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -682,7 +643,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -694,299 +655,61 @@
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="4">
+        <v>100.0</v>
+      </c>
       <c r="M8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="4">
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="J9" s="4">
+        <v>97.5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>85.2</v>
+      </c>
       <c r="L9" s="4">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="4">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="4">
-        <v>25</v>
-      </c>
-      <c r="F10" s="4">
-        <v>3</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4">
-        <v>66.67</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="4">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
-        <v>28</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="4">
-        <v>8</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="4">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="4">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4">
-        <v>22</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="4">
-        <v>100</v>
-      </c>
-      <c r="K14" s="4">
-        <v>95</v>
-      </c>
-      <c r="L14" s="4">
-        <v>100.0</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="4">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4">
-        <v>40</v>
-      </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="4">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4">
-        <v>100</v>
-      </c>
-      <c r="L16" s="4">
-        <v>100.0</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="4">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="4">
-        <v>97.5</v>
-      </c>
-      <c r="K17" s="4">
-        <v>85.2</v>
-      </c>
-      <c r="L17" s="4">
-        <v>80.0</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N17" s="4">
         <v>5</v>
       </c>
     </row>
@@ -994,9 +717,7 @@
   <mergeCells>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
-    <mergeCell ref="D5:D9"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>